<commit_message>
Update final para pedir a placa
O C10 não tinha na JLC ai coloquei outro
</commit_message>
<xml_diff>
--- a/teclado/Project Outputs for teclado/Bill of Materials/Teclas not fitted.xlsx
+++ b/teclado/Project Outputs for teclado/Bill of Materials/Teclas not fitted.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitor\AppData\Local\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuel-my.sharepoint.com/personal/vitor_hugo_domingues_bogo_live_uel_br/Documents/[1]-Pcompartilhada/[3]-3_ano/PI 3B/altium/Grupo4-TecladoNumerico/teclado/Project Outputs for teclado/Bill of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5ED4CDE9-CD68-4C78-A59E-A3F54E7E9E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{573C0CBF-9D4B-45BB-8EAE-03F8FD43D80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8914532-7DD3-4A81-A60F-0A86A0A92268}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{904067F2-9376-4794-A359-95377ED8565D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB52BDB4-E166-468B-86BA-56C00564DC21}"/>
   </bookViews>
   <sheets>
     <sheet name="Teclas not fitted" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="118">
   <si>
     <t>Line #</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>LibRef</t>
-  </si>
-  <si>
     <t>Supplier Part Number</t>
   </si>
   <si>
@@ -155,31 +152,28 @@
     <t>Vishay</t>
   </si>
   <si>
-    <t>0201 22 nF 6.3 V ±10% Tolerance X5R SMT Multilayer Ceramic Capacitor</t>
+    <t>Ceramic Capacitor, Multilayer, Ceramic, 50V, 5% +Tol, 5% -Tol, C0G, 0+-30ppm/Celcius TC, 33pF, Surface Mount, 0402 inch</t>
+  </si>
+  <si>
+    <t>C6, C7</t>
+  </si>
+  <si>
+    <t>CL05C330JB5NNNC</t>
+  </si>
+  <si>
+    <t>1276-1272-1-ND</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor, Multilayer, Ceramic, 50V, 10% +Tol, 10% -Tol, X7R, +-15% TC, 22nF, Surface Mount, 0603 inch</t>
   </si>
   <si>
     <t>C10</t>
   </si>
   <si>
-    <t>GRM033R60J223KE01D</t>
-  </si>
-  <si>
-    <t>490-3169-1-ND</t>
-  </si>
-  <si>
-    <t>Murata</t>
-  </si>
-  <si>
-    <t>Ceramic Capacitor, Multilayer, Ceramic, 50V, 5% +Tol, 5% -Tol, C0G, 0+-30ppm/Celcius TC, 33pF, Surface Mount, 0402 inch</t>
-  </si>
-  <si>
-    <t>C6, C7</t>
-  </si>
-  <si>
-    <t>CL05C330JB5NNNC</t>
-  </si>
-  <si>
-    <t>1276-1272-1-ND</t>
+    <t>CL10B223KB8WPNC</t>
+  </si>
+  <si>
+    <t>1276-6534-1-ND</t>
   </si>
   <si>
     <t>Conn Shrouded Header (4 Sides) HDR 20 POS 2.54mm Solder ST Top Entry Thru-Hole</t>
@@ -396,6 +390,9 @@
   </si>
   <si>
     <t>Bourns</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -791,10 +788,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065653DF-340F-41C2-AD99-D2269C33E539}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5609FB-C1DE-4AA0-B2C9-0AC700EABD9D}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -831,66 +830,66 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="G2" s="1">
         <v>0.01</v>
@@ -899,28 +898,28 @@
         <v>3746544</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1">
         <v>10</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="Q2" s="1">
         <v>5.0000000000000001E-3</v>
@@ -931,52 +930,52 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D3" s="1">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="G3" s="1">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>5839005</v>
+        <v>5838018</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="1">
         <v>10</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="Q3" s="1">
         <v>6.0000000000000001E-3</v>
@@ -987,52 +986,52 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D4" s="1">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="G4" s="1">
         <v>0.24</v>
       </c>
       <c r="H4" s="1">
-        <v>3294276</v>
+        <v>3238174</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" s="1">
         <v>10</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="Q4" s="1">
         <v>0.03</v>
@@ -1043,132 +1042,130 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="G5" s="1">
-        <v>0.1</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H5" s="1">
-        <v>1612421</v>
+        <v>3172986</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="1">
+        <v>10</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="1">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="M5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="Q5" s="1">
-        <v>0.1</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="R5" s="1">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="G6" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="H6" s="1">
-        <v>3172986</v>
+        <v>843417</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="1">
-        <v>10</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="R6" s="1">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="G7" s="1">
         <v>0.41</v>
@@ -1177,28 +1174,28 @@
         <v>30037</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J7" s="1">
         <v>1</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q7" s="1">
         <v>0.41</v>
@@ -1209,22 +1206,22 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="G8" s="1">
         <v>0.44</v>
@@ -1233,28 +1230,28 @@
         <v>4142</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="1">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="L8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P8" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Q8" s="1">
         <v>0.44</v>
@@ -1265,22 +1262,22 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1">
         <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G9" s="1">
         <v>0.91500000000000004</v>
@@ -1289,28 +1286,28 @@
         <v>1059989</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" s="1">
         <v>15</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P9" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Q9" s="1">
         <v>6.0999999999999999E-2</v>
@@ -1321,22 +1318,22 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="G10" s="1">
         <v>0.28999999999999998</v>
@@ -1345,28 +1342,28 @@
         <v>236143</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="1">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="L10" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P10" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q10" s="1">
         <v>0.28999999999999998</v>
@@ -1377,52 +1374,52 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1">
         <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G11" s="1">
         <v>74.25</v>
       </c>
       <c r="H11" s="1">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J11" s="1">
         <v>15</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q11" s="1">
         <v>4.95</v>
@@ -1434,19 +1431,19 @@
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="G12" s="1">
         <v>6.08</v>
@@ -1455,28 +1452,28 @@
         <v>3958</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J12" s="1">
         <v>1</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q12" s="1">
         <v>6.08</v>
@@ -1487,22 +1484,22 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="G13" s="1">
         <v>0.08</v>
@@ -1511,28 +1508,28 @@
         <v>926448</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="1">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="L13" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O13" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P13" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q13" s="1">
         <v>0.08</v>
@@ -1543,22 +1540,22 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G14" s="1">
         <v>0.2</v>
@@ -1567,28 +1564,28 @@
         <v>142982</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J14" s="1">
         <v>2</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O14" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P14" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q14" s="1">
         <v>0.1</v>
@@ -1599,22 +1596,22 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="G15" s="1">
         <v>0.1</v>
@@ -1623,28 +1620,28 @@
         <v>157239</v>
       </c>
       <c r="I15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="1">
-        <v>1</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="L15" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O15" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P15" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q15" s="1">
         <v>0.1</v>
@@ -1656,19 +1653,19 @@
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="G16" s="1">
         <v>0.1</v>
@@ -1677,28 +1674,28 @@
         <v>105630</v>
       </c>
       <c r="I16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="1">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="L16" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O16" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P16" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q16" s="1">
         <v>0.1</v>
@@ -1709,22 +1706,22 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="G17" s="1">
         <v>0.41</v>
@@ -1733,28 +1730,28 @@
         <v>17489</v>
       </c>
       <c r="I17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="1">
-        <v>1</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="L17" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q17" s="1">
         <v>0.41</v>
@@ -1765,22 +1762,22 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="G18" s="1">
         <v>1.24</v>
@@ -1789,28 +1786,28 @@
         <v>27309</v>
       </c>
       <c r="I18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="1">
-        <v>1</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="L18" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O18" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P18" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q18" s="1">
         <v>1.24</v>
@@ -1821,22 +1818,22 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="G19" s="1">
         <v>0.36</v>
@@ -1845,28 +1842,28 @@
         <v>63702</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="1">
-        <v>1</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="L19" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O19" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P19" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Q19" s="1">
         <v>0.36</v>
@@ -1877,22 +1874,22 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G20" s="1">
         <v>0.2</v>
@@ -1901,28 +1898,28 @@
         <v>158716</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J20" s="1">
         <v>2</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O20" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="P20" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q20" s="1">
         <v>0.1</v>

</xml_diff>

<commit_message>
Corrigindo componentes e etc
-diodos trocados pelos sugeridos
-conector trocado, por um conector angulado
-furos da borda alinhados) agora estão com todos estão com 4mm de distancia das bordas)
-componentes da usb realinhados(acho que assim fica melhor)
-arrumei as ligações duplas da usb usando áreas.

*nota, não troquei o usb, o que foi sugerido não tinha pinos o suficientes

-os arquivos de output para gerar a pcb estão atualizados
</commit_message>
<xml_diff>
--- a/teclado/Project Outputs for teclado/Bill of Materials/Teclas not fitted.xlsx
+++ b/teclado/Project Outputs for teclado/Bill of Materials/Teclas not fitted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuel-my.sharepoint.com/personal/vitor_hugo_domingues_bogo_live_uel_br/Documents/[1]-Pcompartilhada/[3]-3_ano/PI 3B/altium/Grupo4-TecladoNumerico/teclado/Project Outputs for teclado/Bill of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{FB4DB57C-66EA-456A-9134-FA25EA11878A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4682BDBA-C726-4429-8981-44DE817BA908}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{7E661036-07DD-4C5C-BBD7-6E251CFD366C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82F6B54D-6871-485C-B115-E996AFC67500}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0624E8E3-C601-4D94-8E00-A6F9292EB2B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B2228A7-BC45-482E-8A9A-2D2E83AD272E}"/>
   </bookViews>
   <sheets>
     <sheet name="Teclas not fitted" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="111">
   <si>
     <t>Line #</t>
   </si>
@@ -98,7 +98,7 @@
     <t>10V 1uF X7R ±10% 0603 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
-    <t>C5, C8</t>
+    <t>C9, C14</t>
   </si>
   <si>
     <t>CL10B105KP8NNNC</t>
@@ -125,7 +125,7 @@
     <t>16V 100nF X7R ±10% 0603 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4, C9, C12, C13</t>
+    <t>C1, C3, C4, C5, C6, C7, C10, C13</t>
   </si>
   <si>
     <t>CC0603KRX7R7BB104</t>
@@ -140,7 +140,7 @@
     <t>100Mw Thick Film Resistors 100Ppm/ 5% 1.5K 0603 Chip Resistor Surface Mount Rohs</t>
   </si>
   <si>
-    <t>R1</t>
+    <t>R3</t>
   </si>
   <si>
     <t>RC0603JR-071K5L</t>
@@ -152,7 +152,7 @@
     <t>100mW Thick Film Resistors ±1% ±100ppm/℃ 10kΩ 0603 Chip Resistor - Surface Mount ROHS</t>
   </si>
   <si>
-    <t>R2, R4, R9, R10, R11, R12, R13, R14</t>
+    <t>R5, R6, R7, R8, R9, R10, R11, R12</t>
   </si>
   <si>
     <t>CRCW060310K0FKEA</t>
@@ -167,7 +167,7 @@
     <t>0603 27 pF 50 V ±1 % Tolerance NP0 SMT Multilayer Ceramic Capacitor</t>
   </si>
   <si>
-    <t>C6, C7</t>
+    <t>C2, C8</t>
   </si>
   <si>
     <t>CC0603FRNPO9BN270</t>
@@ -179,7 +179,7 @@
     <t>Ceramic Capacitor, Multilayer, Ceramic, 50V, 10% +Tol, 10% -Tol, X7R, +-15% TC, 22nF, Surface Mount, 0603 inch</t>
   </si>
   <si>
-    <t>C10</t>
+    <t>C11</t>
   </si>
   <si>
     <t>CL10B223KB8WPNC</t>
@@ -188,136 +188,136 @@
     <t>1276-6534-1-ND</t>
   </si>
   <si>
-    <t>Conn Shrouded Header (4 Sides) HDR 20 POS 2.54mm Solder ST Top Entry Thru-Hole</t>
+    <t>Conn Shrouded Header (4 Sides) HDR 20 POS 2.54mm Solder RA Side Entry Thru-HoleC-Grid Tray</t>
   </si>
   <si>
     <t>J1</t>
   </si>
   <si>
-    <t>SBH11-PBPC-D10-ST-BK</t>
-  </si>
-  <si>
-    <t>S9172-ND</t>
+    <t>70247-2051</t>
+  </si>
+  <si>
+    <t>23-0702472051-ND</t>
+  </si>
+  <si>
+    <t>Bulk</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>Crystal 8MHz ±30ppm (Tol) ±100ppm (Stability) 20pF FUND 60Ohm 2-Pin SMD T/R</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ECS-80-20-5PXDU-TR</t>
+  </si>
+  <si>
+    <t>XC1526CT-ND</t>
+  </si>
+  <si>
+    <t>ECS International</t>
+  </si>
+  <si>
+    <t>Fuse Chip Fast Acting 0.5A 32V SMD Solder Pad 0603 1.6 X 0.8 X 0.54mm T/R UL/cUL</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>ERB-RE0R50V</t>
+  </si>
+  <si>
+    <t>P15127CT-ND</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>GENERAL PURPOSE CHIP RESISTOR Metal Glaze/thick Film, 0.1W, 0ohm, Surface Mount, 0603</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>RC0603JR-070RL</t>
+  </si>
+  <si>
+    <t>311-0.0GRCT-ND</t>
+  </si>
+  <si>
+    <t>Kailh Switch Sockets For Mx-Compatible Mechanical Keys - 20 Pack |Adafruit 4958</t>
+  </si>
+  <si>
+    <t>U2, U3, U4, U6, U7, U8, U9, U10, U11, U12, U13, U14, U16, U17, U18</t>
+  </si>
+  <si>
+    <t>4958</t>
+  </si>
+  <si>
+    <t>1528-4958-ND</t>
+  </si>
+  <si>
+    <t>Adafruit Industries</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>MCU 32-bit STM32F1 ARM Cortex M3 RISC 64KB Flash 2.5V/3.3V 48-Pin LQFP Tray</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>STM32F103C8T6</t>
+  </si>
+  <si>
+    <t>497-6063-ND</t>
   </si>
   <si>
     <t>Tray</t>
   </si>
   <si>
-    <t>Sullins</t>
-  </si>
-  <si>
-    <t>Crystal 8MHz ±30ppm (Tol) ±100ppm (Stability) 20pF FUND 60Ohm 2-Pin SMD T/R</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ECS-80-20-5PXDU-TR</t>
-  </si>
-  <si>
-    <t>XC1526CT-ND</t>
-  </si>
-  <si>
-    <t>ECS International</t>
-  </si>
-  <si>
-    <t>Diode, Rectifier, Fast, Vr 100V, If 300MA, Pkg SOD-323, Vf 1V, Trr 4NS, Cj 4PF, Tj +150C</t>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors (High dielectric type), 10V, 10 uF, ± 20 %, 0603, X5R, RoHS</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>LMK107BBJ106MALT</t>
+  </si>
+  <si>
+    <t>587-3258-1-ND</t>
+  </si>
+  <si>
+    <t>TAIYO YUDEN</t>
+  </si>
+  <si>
+    <t>Rectifier Diode Schottky 40V 0.03A 2-Pin SOD-323 T/R / DIODE SCHOTTKY 30V 30MA SOD323</t>
   </si>
   <si>
     <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15</t>
   </si>
   <si>
-    <t>1N4148WX-TP</t>
-  </si>
-  <si>
-    <t>1N4148WXTPMSCT-ND</t>
-  </si>
-  <si>
-    <t>MCC</t>
-  </si>
-  <si>
-    <t>Fuse Chip Fast Acting 0.5A 32V SMD Solder Pad 0603 1.6 X 0.8 X 0.54mm T/R UL/cUL</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>ERB-RE0R50V</t>
-  </si>
-  <si>
-    <t>P15127CT-ND</t>
-  </si>
-  <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
-    <t>GENERAL PURPOSE CHIP RESISTOR Metal Glaze/thick Film, 0.1W, 0ohm, Surface Mount, 0603</t>
-  </si>
-  <si>
-    <t>R3, R5</t>
-  </si>
-  <si>
-    <t>RC0603JR-070RL</t>
-  </si>
-  <si>
-    <t>311-0.0GRCT-ND</t>
-  </si>
-  <si>
-    <t>Kailh Switch Sockets For Mx-Compatible Mechanical Keys - 20 Pack |Adafruit 4958</t>
-  </si>
-  <si>
-    <t>U2, U3, U4, U6, U7, U8, U9, U10, U11, U12, U13, U14, U15, U16, U17</t>
-  </si>
-  <si>
-    <t>4958</t>
-  </si>
-  <si>
-    <t>1528-4958-ND</t>
-  </si>
-  <si>
-    <t>Bulk</t>
-  </si>
-  <si>
-    <t>Adafruit Industries</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>MCU 32-bit STM32F1 ARM Cortex M3 RISC 64KB Flash 2.5V/3.3V 48-Pin LQFP Tray</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>STM32F103C8T6</t>
-  </si>
-  <si>
-    <t>497-6063-ND</t>
-  </si>
-  <si>
-    <t>STMicroelectronics</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors (High dielectric type), 10V, 10 uF, ± 20 %, 0603, X5R, RoHS</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>LMK107BBJ106MALT</t>
-  </si>
-  <si>
-    <t>587-3258-1-ND</t>
-  </si>
-  <si>
-    <t>TAIYO YUDEN</t>
+    <t>RB751V40T1G</t>
+  </si>
+  <si>
+    <t>RB751V40T1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>onsemi</t>
   </si>
   <si>
     <t>Res Thick Film 0603 5.1K Ohm 1% 0.1W(1/10W) ±100ppm/C Pad SMD T/R</t>
   </si>
   <si>
-    <t>R6, R7</t>
+    <t>R1, R2</t>
   </si>
   <si>
     <t>RC0603FR-075K1L</t>
@@ -338,18 +338,12 @@
     <t>1028-1014-1-ND</t>
   </si>
   <si>
-    <t>Tape &amp; Reel</t>
-  </si>
-  <si>
     <t>Richtek</t>
   </si>
   <si>
     <t>Obsolete</t>
   </si>
   <si>
-    <t>1028-1014-2-ND</t>
-  </si>
-  <si>
     <t>USB Connector, 16 Contact(s), Male, Right Angle, Surface Mount Terminal, Locking, Receptacle</t>
   </si>
   <si>
@@ -368,7 +362,7 @@
     <t>USBLC6 Series 2 Line 6 V Uni / Bi-Directional ESD Protection - SOT-23-6</t>
   </si>
   <si>
-    <t>U18</t>
+    <t>U15</t>
   </si>
   <si>
     <t>USBLC6-2SC6</t>
@@ -782,11 +776,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4622AC28-2006-4A30-AB2C-4A943134514F}">
-  <dimension ref="A1:R21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20D8CD3-A462-4354-8762-2214A3E8AF66}">
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -824,7 +818,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -889,7 +883,7 @@
         <v>0.01</v>
       </c>
       <c r="H2" s="1">
-        <v>3562122</v>
+        <v>3540967</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>22</v>
@@ -933,7 +927,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>29</v>
@@ -942,10 +936,10 @@
         <v>30</v>
       </c>
       <c r="G3" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>5646284</v>
+        <v>5424503</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>22</v>
@@ -999,7 +993,7 @@
         <v>0.1</v>
       </c>
       <c r="H4" s="1">
-        <v>699035</v>
+        <v>687335</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>22</v>
@@ -1055,7 +1049,7 @@
         <v>0.24</v>
       </c>
       <c r="H5" s="1">
-        <v>2957755</v>
+        <v>2856834</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>22</v>
@@ -1165,7 +1159,7 @@
         <v>0.1</v>
       </c>
       <c r="H7" s="1">
-        <v>841992</v>
+        <v>841892</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>22</v>
@@ -1216,10 +1210,10 @@
         <v>52</v>
       </c>
       <c r="G8" s="1">
-        <v>0.41</v>
+        <v>3.89</v>
       </c>
       <c r="H8" s="1">
-        <v>38143</v>
+        <v>2615</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>53</v>
@@ -1246,10 +1240,10 @@
         <v>52</v>
       </c>
       <c r="Q8" s="1">
-        <v>0.41</v>
+        <v>3.89</v>
       </c>
       <c r="R8" s="1">
-        <v>0.41</v>
+        <v>3.89</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -1275,7 +1269,7 @@
         <v>0.45</v>
       </c>
       <c r="H9" s="1">
-        <v>7442</v>
+        <v>7422</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>22</v>
@@ -1309,9 +1303,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>60</v>
       </c>
@@ -1319,7 +1311,7 @@
         <v>61</v>
       </c>
       <c r="D10" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>62</v>
@@ -1328,16 +1320,16 @@
         <v>63</v>
       </c>
       <c r="G10" s="1">
-        <v>0.91500000000000004</v>
+        <v>0.31</v>
       </c>
       <c r="H10" s="1">
-        <v>989460</v>
+        <v>2919</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J10" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>23</v>
@@ -1358,10 +1350,10 @@
         <v>63</v>
       </c>
       <c r="Q10" s="1">
-        <v>6.0999999999999999E-2</v>
+        <v>0.31</v>
       </c>
       <c r="R10" s="1">
-        <v>0.91500000000000004</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -1382,10 +1374,10 @@
         <v>68</v>
       </c>
       <c r="G11" s="1">
-        <v>0.32</v>
+        <v>0.1</v>
       </c>
       <c r="H11" s="1">
-        <v>103995</v>
+        <v>2939930</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>22</v>
@@ -1397,7 +1389,7 @@
         <v>23</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>67</v>
@@ -1412,10 +1404,10 @@
         <v>68</v>
       </c>
       <c r="Q11" s="1">
-        <v>0.32</v>
+        <v>0.1</v>
       </c>
       <c r="R11" s="1">
-        <v>0.32</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -1423,115 +1415,115 @@
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="1">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="G12" s="1">
-        <v>0.02</v>
+        <v>74.25</v>
       </c>
       <c r="H12" s="1">
-        <v>3032959</v>
+        <v>37</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="J12" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q12" s="1">
-        <v>0.01</v>
+        <v>4.95</v>
       </c>
       <c r="R12" s="1">
-        <v>0.1</v>
+        <v>74.25</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D13" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G13" s="1">
-        <v>74.25</v>
+        <v>6.08</v>
       </c>
       <c r="H13" s="1">
-        <v>52</v>
+        <v>3373</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J13" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Q13" s="1">
-        <v>4.95</v>
+        <v>6.08</v>
       </c>
       <c r="R13" s="1">
-        <v>74.25</v>
+        <v>6.08</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>81</v>
       </c>
@@ -1548,13 +1540,13 @@
         <v>84</v>
       </c>
       <c r="G14" s="1">
-        <v>6.08</v>
+        <v>0.08</v>
       </c>
       <c r="H14" s="1">
-        <v>3673</v>
+        <v>861176</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="J14" s="1">
         <v>1</v>
@@ -1578,10 +1570,10 @@
         <v>84</v>
       </c>
       <c r="Q14" s="1">
-        <v>6.08</v>
+        <v>0.08</v>
       </c>
       <c r="R14" s="1">
-        <v>6.08</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -1595,7 +1587,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>88</v>
@@ -1604,16 +1596,16 @@
         <v>89</v>
       </c>
       <c r="G15" s="1">
-        <v>0.08</v>
+        <v>1.2</v>
       </c>
       <c r="H15" s="1">
-        <v>862284</v>
+        <v>326728</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>23</v>
@@ -1637,7 +1629,7 @@
         <v>0.08</v>
       </c>
       <c r="R15" s="1">
-        <v>0.08</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1663,7 +1655,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="H16" s="1">
-        <v>635309</v>
+        <v>618540</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>22</v>
@@ -1715,67 +1707,49 @@
       <c r="F17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="1">
-        <v>0.17732000000000001</v>
-      </c>
-      <c r="H17" s="1">
-        <v>15000</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="J17" s="1">
-        <v>3000</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>97</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>0.17732000000000001</v>
-      </c>
-      <c r="R17" s="1">
-        <v>531.96</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="G18" s="1">
         <v>1.23</v>
       </c>
       <c r="H18" s="1">
-        <v>12995</v>
+        <v>38043</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>22</v>
@@ -1787,10 +1761,10 @@
         <v>23</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>25</v>
@@ -1799,7 +1773,7 @@
         <v>26</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Q18" s="1">
         <v>1.23</v>
@@ -1813,25 +1787,25 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="G19" s="1">
         <v>0.36</v>
       </c>
       <c r="H19" s="1">
-        <v>144005</v>
+        <v>126022</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>22</v>
@@ -1843,10 +1817,10 @@
         <v>23</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>25</v>
@@ -1855,7 +1829,7 @@
         <v>26</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q19" s="1">
         <v>0.36</v>
@@ -1864,8 +1838,8 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E21" s="5"/>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E22" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>